<commit_message>
changes in look of the website
</commit_message>
<xml_diff>
--- a/book_data.xlsx
+++ b/book_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayt\Desktop\LocalLibrary\LocalLibrary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D412C6F3-2035-491B-8E12-5826FD4F6F5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6834EA69-10E2-4D15-8594-8EA405C79B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="115">
   <si>
     <t>Sr No.</t>
   </si>
@@ -254,9 +254,6 @@
     <t>978-9-38-162681-8</t>
   </si>
   <si>
-    <t>Thriller</t>
-  </si>
-  <si>
     <t>Chanakya's Chant</t>
   </si>
   <si>
@@ -494,6 +491,39 @@
   </si>
   <si>
     <t>978-81-929109-0-1</t>
+  </si>
+  <si>
+    <t>Thriller, Historical Fiction, Suspense</t>
+  </si>
+  <si>
+    <t>Mystery, Crime Fiction, Thriller</t>
+  </si>
+  <si>
+    <t>Mystery, Thriller, Conspiracy Fiction</t>
+  </si>
+  <si>
+    <t>Crime Fiction, Thriller, Suspense, Conspiracy Fiction</t>
+  </si>
+  <si>
+    <t>Mystery, Conspiracy Fiction, Detective Fiction, Thriller</t>
+  </si>
+  <si>
+    <t>Mystery, Fiction, Thriller</t>
+  </si>
+  <si>
+    <t>Mystery, Children's Literature</t>
+  </si>
+  <si>
+    <t>Sherlock Holmes is intrigued by a centuries-old legend in which every generation of the wealthy Baskerville family is eventually killed by a monstrous hound. Suspecting there is more to the story than meets the eye, he sends Dr. Watson to the estate to investigate. Sir Henry, the only Baskerville left, is grateful for his help. But when a crazed convict escapes and footprints from a beast are found, Baskerville wonders if Watson will be enough.</t>
+  </si>
+  <si>
+    <t>Fiction, Politics, Romance</t>
+  </si>
+  <si>
+    <t>Fable, Fiction</t>
+  </si>
+  <si>
+    <t>Science Fiction, Alternate History, Social Science Fiction, Political Fiction, Dystopian Fiction</t>
   </si>
 </sst>
 </file>
@@ -842,7 +872,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +1237,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>65</v>
@@ -1216,27 +1246,30 @@
         <v>66</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:6" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -1244,17 +1277,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -1262,17 +1297,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="4" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -1280,17 +1317,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -1298,17 +1337,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1316,33 +1357,39 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1350,17 +1397,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -1368,17 +1417,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="4" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -1389,14 +1440,16 @@
         <v>1984</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>